<commit_message>
backlog updates to csv
</commit_message>
<xml_diff>
--- a/backlog1.xlsx
+++ b/backlog1.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" r:id="rId1"/>
-    <sheet name="Definition of done" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>ID</t>
   </si>
@@ -174,18 +173,6 @@
   </si>
   <si>
     <t>p</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>definition of done</t>
-  </si>
-  <si>
-    <t>when I can login in with a username and password and be able to select options to either start or continue a game</t>
-  </si>
-  <si>
-    <t xml:space="preserve">when I can select the level and category of game and be able to start playing </t>
   </si>
 </sst>
 </file>
@@ -201,18 +188,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,20 +208,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -266,9 +246,9 @@
   <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="3" name="As a/an"/>
-    <tableColumn id="4" name="I want to…" dataDxfId="1"/>
-    <tableColumn id="5" name="so that.."/>
-    <tableColumn id="6" name="Notes " dataDxfId="0"/>
+    <tableColumn id="4" name="I want to…" dataDxfId="2"/>
+    <tableColumn id="5" name="so that.." dataDxfId="0"/>
+    <tableColumn id="6" name="Notes " dataDxfId="1"/>
     <tableColumn id="7" name="Priority"/>
     <tableColumn id="8" name="Estimation"/>
     <tableColumn id="9" name="Status"/>
@@ -567,7 +547,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,11 +555,11 @@
     <col min="1" max="1" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.453125" customWidth="1"/>
     <col min="3" max="3" width="40.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7265625" customWidth="1"/>
-    <col min="5" max="5" width="15.1796875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" customWidth="1"/>
     <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -592,7 +572,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -688,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -857,7 +837,7 @@
       <c r="C15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
@@ -910,91 +890,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="16.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="37.7265625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
commit -a -m 'plugins'
</commit_message>
<xml_diff>
--- a/backlog1.xlsx
+++ b/backlog1.xlsx
@@ -217,7 +217,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -241,13 +244,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H1048576" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:H1048576"/>
   <tableColumns count="8">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="3" name="As a/an"/>
-    <tableColumn id="4" name="I want to…" dataDxfId="2"/>
-    <tableColumn id="5" name="so that.." dataDxfId="0"/>
+    <tableColumn id="4" name="I want to…" dataDxfId="3"/>
+    <tableColumn id="5" name="so that.." dataDxfId="2"/>
     <tableColumn id="6" name="Notes " dataDxfId="1"/>
     <tableColumn id="7" name="Priority"/>
     <tableColumn id="8" name="Estimation"/>
@@ -547,26 +550,26 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.453125" customWidth="1"/>
-    <col min="3" max="3" width="40.90625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" customWidth="1"/>
-    <col min="7" max="7" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.90625" customWidth="1"/>
+    <col min="3" max="3" width="32.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" customWidth="1"/>
+    <col min="8" max="8" width="6.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -578,17 +581,17 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>

</xml_diff>